<commit_message>
add sesiones y dispositivos
</commit_message>
<xml_diff>
--- a/api/db/sesion_3001.xlsx
+++ b/api/db/sesion_3001.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alienware\Desktop\Proyectos software\EOLO_WEBAPP\api\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DREAMFYRE 5\Desktop\Proyectos\EOLO_WEBAPP\api\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190BF871-4E94-4B55-A008-916BA913B661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD5FE56-3BAE-402A-8429-BEF0935B6EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="14">
-  <si>
-    <t>dispositivo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="10">
   <si>
     <t>sesion_id</t>
-  </si>
-  <si>
-    <t>modelo</t>
   </si>
   <si>
     <t>dia</t>
@@ -45,28 +39,22 @@
     <t>año</t>
   </si>
   <si>
-    <t>Eolo_MP_300</t>
-  </si>
-  <si>
-    <t>Modelo 3.0</t>
-  </si>
-  <si>
     <t>valor</t>
   </si>
   <si>
     <t>variable</t>
   </si>
   <si>
-    <t>% co2</t>
-  </si>
-  <si>
     <t>timestamp</t>
   </si>
   <si>
-    <t>ubicacion</t>
+    <t>patente</t>
   </si>
   <si>
-    <t>Santiago, Chile</t>
+    <t>°C</t>
+  </si>
+  <si>
+    <t>MP-01-EXPRESS</t>
   </si>
 </sst>
 </file>
@@ -391,54 +379,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
       <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>3001</v>
@@ -456,21 +437,15 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2">
+        <v>8</v>
+      </c>
+      <c r="H2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>3001</v>
@@ -488,21 +463,15 @@
         <v>0.83333333333333304</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3">
+        <v>8</v>
+      </c>
+      <c r="H3">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>3001</v>
@@ -520,21 +489,15 @@
         <v>0.875</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4">
+        <v>8</v>
+      </c>
+      <c r="H4">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>3001</v>
@@ -552,21 +515,15 @@
         <v>0.91666666666666696</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5">
+        <v>8</v>
+      </c>
+      <c r="H5">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>3001</v>
@@ -584,21 +541,15 @@
         <v>0.95833333333333304</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6">
         <v>10</v>
       </c>
-      <c r="J6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>3001</v>
@@ -616,21 +567,15 @@
         <v>0.999999999999999</v>
       </c>
       <c r="G7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7">
+        <v>8</v>
+      </c>
+      <c r="H7">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>3001</v>
@@ -648,21 +593,15 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8">
+        <v>8</v>
+      </c>
+      <c r="H8">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>3001</v>
@@ -680,21 +619,15 @@
         <v>8.3333333333338894E-2</v>
       </c>
       <c r="G9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="H9">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>3001</v>
@@ -712,21 +645,15 @@
         <v>0.124999999999999</v>
       </c>
       <c r="G10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10">
+        <v>8</v>
+      </c>
+      <c r="H10">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>3001</v>
@@ -744,21 +671,15 @@
         <v>0.16666666666666899</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11">
+        <v>8</v>
+      </c>
+      <c r="H11">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B12">
         <v>3001</v>
@@ -776,21 +697,15 @@
         <v>0.208333333333339</v>
       </c>
       <c r="G12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12">
+        <v>8</v>
+      </c>
+      <c r="H12">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B13">
         <v>3001</v>
@@ -808,21 +723,15 @@
         <v>0.25000000000000899</v>
       </c>
       <c r="G13" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" t="s">
-        <v>7</v>
-      </c>
-      <c r="I13" t="s">
-        <v>10</v>
-      </c>
-      <c r="J13">
+        <v>8</v>
+      </c>
+      <c r="H13">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B14">
         <v>3001</v>
@@ -840,21 +749,15 @@
         <v>0.29166666666666902</v>
       </c>
       <c r="G14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J14">
+        <v>8</v>
+      </c>
+      <c r="H14">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B15">
         <v>3001</v>
@@ -872,21 +775,15 @@
         <v>0.33333333333333898</v>
       </c>
       <c r="G15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" t="s">
-        <v>7</v>
-      </c>
-      <c r="I15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J15">
+        <v>8</v>
+      </c>
+      <c r="H15">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B16">
         <v>3001</v>
@@ -904,21 +801,15 @@
         <v>0.37500000000000999</v>
       </c>
       <c r="G16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" t="s">
-        <v>7</v>
-      </c>
-      <c r="I16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J16">
+        <v>8</v>
+      </c>
+      <c r="H16">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B17">
         <v>3001</v>
@@ -936,21 +827,15 @@
         <v>0.41666666666667901</v>
       </c>
       <c r="G17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" t="s">
-        <v>7</v>
-      </c>
-      <c r="I17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17">
         <v>10</v>
       </c>
-      <c r="J17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B18">
         <v>3001</v>
@@ -968,21 +853,15 @@
         <v>0.45833333333329801</v>
       </c>
       <c r="G18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" t="s">
-        <v>7</v>
-      </c>
-      <c r="I18" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18">
+        <v>8</v>
+      </c>
+      <c r="H18">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B19">
         <v>3001</v>
@@ -1000,21 +879,15 @@
         <v>0.499999999999998</v>
       </c>
       <c r="G19" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" t="s">
-        <v>7</v>
-      </c>
-      <c r="I19" t="s">
-        <v>10</v>
-      </c>
-      <c r="J19">
+        <v>8</v>
+      </c>
+      <c r="H19">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B20">
         <v>3001</v>
@@ -1032,15 +905,9 @@
         <v>0.54166666666669805</v>
       </c>
       <c r="G20" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" t="s">
-        <v>7</v>
-      </c>
-      <c r="I20" t="s">
-        <v>10</v>
-      </c>
-      <c r="J20">
+        <v>8</v>
+      </c>
+      <c r="H20">
         <v>30</v>
       </c>
     </row>

</xml_diff>